<commit_message>
Updated Milestone 2 SCRUM content.
</commit_message>
<xml_diff>
--- a/Documentation/Scrum/Sprint1Backlog.xlsx
+++ b/Documentation/Scrum/Sprint1Backlog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ali\Documents\cst247\Documentation\Scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caleb Ljunggren\Documents\School (GCU)\CST-247\Bitbucket-GitHub\Documentation\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Use Case Template" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Project Title: Minesweeper
 Release #: 1.0.0
@@ -92,12 +92,15 @@
   </si>
   <si>
     <t>Ali Cooper</t>
+  </si>
+  <si>
+    <t>Caleb Ljunggren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -230,12 +233,6 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,6 +264,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,174 +583,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="42.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="1" customWidth="1"/>
     <col min="8" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="1" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="6"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>0</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F4">
         <v>4</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>21</v>
+      <c r="G5" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
       <c r="C7"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8"/>
       <c r="D8"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
       <c r="C9"/>
       <c r="D9"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="9"/>
       <c r="D10"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>